<commit_message>
removed duplicate inlfuencers 2
</commit_message>
<xml_diff>
--- a/ESERCIZIO_M2-2-3_dati.xlsx
+++ b/ESERCIZIO_M2-2-3_dati.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leona\Desktop\EPICODE\W2\Esercizio pratica\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leona\Desktop\EPICODE\Git\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A3AF17D-2CA6-47C7-9D27-17072FA2BAEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17F53976-A58E-46BB-9A02-2C1FA488CB29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31957,6 +31957,26 @@
     <dataField name="Somma di VENDITE" fld="2" baseField="0" baseItem="0" numFmtId="165"/>
   </dataFields>
   <conditionalFormats count="2">
+    <conditionalFormat priority="2">
+      <pivotAreas count="1">
+        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="2">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="0" count="7">
+              <x v="0"/>
+              <x v="1"/>
+              <x v="2"/>
+              <x v="3"/>
+              <x v="4"/>
+              <x v="5"/>
+              <x v="6"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
     <conditionalFormat type="all" priority="1">
       <pivotAreas count="1">
         <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
@@ -31984,26 +32004,6 @@
               <x v="7"/>
               <x v="8"/>
               <x v="9"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </pivotAreas>
-    </conditionalFormat>
-    <conditionalFormat priority="2">
-      <pivotAreas count="1">
-        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="2">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="0" count="7">
-              <x v="0"/>
-              <x v="1"/>
-              <x v="2"/>
-              <x v="3"/>
-              <x v="4"/>
-              <x v="5"/>
-              <x v="6"/>
             </reference>
           </references>
         </pivotArea>
@@ -32353,24 +32353,6 @@
     <dataField name="Like + Commenti" fld="10" baseField="9" baseItem="0" numFmtId="1"/>
   </dataFields>
   <conditionalFormats count="2">
-    <conditionalFormat priority="2">
-      <pivotAreas count="1">
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="2">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="2"/>
-            </reference>
-            <reference field="9" count="5">
-              <x v="1"/>
-              <x v="3"/>
-              <x v="4"/>
-              <x v="6"/>
-              <x v="7"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </pivotAreas>
-    </conditionalFormat>
     <conditionalFormat priority="1">
       <pivotAreas count="1">
         <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
@@ -32386,6 +32368,24 @@
               <x v="6"/>
               <x v="7"/>
               <x v="8"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+    <conditionalFormat priority="2">
+      <pivotAreas count="1">
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="2">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="2"/>
+            </reference>
+            <reference field="9" count="5">
+              <x v="1"/>
+              <x v="3"/>
+              <x v="4"/>
+              <x v="6"/>
+              <x v="7"/>
             </reference>
           </references>
         </pivotArea>
@@ -74400,7 +74400,7 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting pivot="1" sqref="D6 D4 D8:D9">
+  <conditionalFormatting pivot="1" sqref="D4 D6 D8:D9">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>